<commit_message>
Modifications des erreurs notées
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="17415" windowHeight="8115"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="17415" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>Catégorie</t>
   </si>
@@ -108,27 +108,6 @@
     <t>Changer le texte alternatif de façon à ce qu'il soit plus clair et qu'il mette la chouette agence en avant sur les pages de Google</t>
   </si>
   <si>
-    <t>Texte alternatif manquant sur la bannière</t>
-  </si>
-  <si>
-    <t>Il manque le texte "alt" sur la bannière, il faut toujours mettre le alt sur les images</t>
-  </si>
-  <si>
-    <t>Peut importe le type ou le format d'image, il est primendial d'ajouter le texte alternatif! D'une part car certains utilisateur ne pourront pas voir cette fameuse image parcequ'ils sont aveugles ou mal voyants, il faut donc utiliser un autre moyen pour ne pas perturber l'experience de ces utilisateurs</t>
-  </si>
-  <si>
-    <t>Rajouter un texte alternatif qui met en avant la chouette agence</t>
-  </si>
-  <si>
-    <t>Texte alternatif manquant sur les logos au dessus de: "web design, stratégie, illustrations"</t>
-  </si>
-  <si>
-    <t>Il manque le texte "alt" sur les logos, il faut toujours mettre le alt sur les logos</t>
-  </si>
-  <si>
-    <t>Peut importe le type ou le format d'image, il est primendial d'ajouter le texte alternatif! D'une part car certains utilisateur ne pourront pas voir cette fameuse image parcequ'ils sont aveugles ou mal voyants, il faut donc utiliser un autre moyen pour ne</t>
-  </si>
-  <si>
     <t xml:space="preserve">L'appel des fichiers JS ne se fais pas correctement. </t>
   </si>
   <si>
@@ -141,9 +120,6 @@
     <t>Ici le mieux serai de faire une exécution "différée" pour que les scripts se lancent dès que le HTML aura finit de se charger</t>
   </si>
   <si>
-    <t>Openclassrooms</t>
-  </si>
-  <si>
     <t>Le temps de chargement du site est trop long</t>
   </si>
   <si>
@@ -192,18 +168,6 @@
     <t>Intégrer les bons mot-clés dans les textes alternatifs</t>
   </si>
   <si>
-    <t>Il manque les textes alternatifs sur les logos sur le Footer bloc-8</t>
-  </si>
-  <si>
-    <t>Si les logos n'ont pas de textes alternatifs cela peut engendrer des problèmes de compréhensions pour les personnes mal voyantes ou voir aveugles.</t>
-  </si>
-  <si>
-    <t>Il faut toujours mettre des textes alternatifs pour les personnes ne pouvant pas visiter votre site web en utilisant leur vue et aussi pour le référencement naturel</t>
-  </si>
-  <si>
-    <t>Ajouter un texte alternatif déscriptif</t>
-  </si>
-  <si>
     <t>Une balise meta n'est pas complétée dans le head de l'index.html</t>
   </si>
   <si>
@@ -228,9 +192,6 @@
     <t>Renseigner la langue du site correctement</t>
   </si>
   <si>
-    <t>Il manque la balise meta "robots index, follow"</t>
-  </si>
-  <si>
     <t>Il manque une balise importante dans le head qui permet aux robots de google d'indexer la page</t>
   </si>
   <si>
@@ -238,13 +199,67 @@
   </si>
   <si>
     <t>Ajouter la balise</t>
+  </si>
+  <si>
+    <t>Il faut remplir la partie "content" sur la balise meta description et keywords sinon le google bot ne pourra pas comprendre</t>
+  </si>
+  <si>
+    <t>Il faut toujours remplir la partie "content" des balises pour augmenter son référencement naturel</t>
+  </si>
+  <si>
+    <t>Les parties "content" des balises keyword et description ne sont pas remplies sur la page2.</t>
+  </si>
+  <si>
+    <t>Il manque la balise meta "robots index, follow" sur l'index et la page2</t>
+  </si>
+  <si>
+    <t>Le texte alternatif du logo de la chouette agence a une mauvaise description</t>
+  </si>
+  <si>
+    <t>Le texte alternatif doit mettre en avant l'agence de lyon et en l'occurrence ici il parle d'atlanta</t>
+  </si>
+  <si>
+    <t>Il faut toujours faire en sorte que le texte alt reprenne les mot-clés pour optimiser le référencement naturel</t>
+  </si>
+  <si>
+    <t>Enlever le "atlanta" par "lyon"</t>
+  </si>
+  <si>
+    <t>La navigation n'est presque pas visible sur la page 2</t>
+  </si>
+  <si>
+    <t>Tout contenu doit être visible pour les visiteurs du site web</t>
+  </si>
+  <si>
+    <t>Recentrer la navigation</t>
+  </si>
+  <si>
+    <t>Reprendre le code CSS pour faire en sorte que la navigation soit au milieu</t>
+  </si>
+  <si>
+    <t>Le site web ne rescpecte pas les normes du W3C validator</t>
+  </si>
+  <si>
+    <t>Il y a des erreurs diverses à  peu près partout sur le site d'ordre sémantique, mauvais emploie de balisage</t>
+  </si>
+  <si>
+    <t>Il faut toujours respecter les normes du W3C car il représente les fondements du web</t>
+  </si>
+  <si>
+    <t>Corriger les erreurs misent en avant par le validateur</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +285,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.45"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -302,10 +323,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,8 +340,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -592,8 +620,11 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>40</v>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
@@ -612,8 +643,11 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>40</v>
+      <c r="F3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
@@ -632,8 +666,11 @@
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>40</v>
+      <c r="F4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
@@ -652,8 +689,11 @@
       <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>40</v>
+      <c r="F5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
@@ -672,48 +712,57 @@
       <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>40</v>
+      <c r="F6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>40</v>
+      <c r="F7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
+      <c r="F8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
@@ -721,19 +770,22 @@
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
@@ -744,21 +796,24 @@
         <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>40</v>
+      <c r="F10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>45</v>
@@ -772,8 +827,11 @@
       <c r="E11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>40</v>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
@@ -792,8 +850,11 @@
       <c r="E12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>40</v>
+      <c r="F12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
@@ -809,31 +870,37 @@
       <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>40</v>
+      <c r="F13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>40</v>
+      <c r="F14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
@@ -841,19 +908,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>40</v>
+      <c r="E15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
@@ -861,56 +931,91 @@
         <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>40</v>
+      <c r="C18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1880,6 +1985,11 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3:F5" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile"/>
+    <hyperlink ref="F6:F18" r:id="rId3" display="https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à jour des références sur le relevé d'erreur
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>Catégorie</t>
   </si>
@@ -253,6 +253,42 @@
   </si>
   <si>
     <t>..</t>
+  </si>
+  <si>
+    <t>https://www.orixa-media.com/academie/referencement-naturel/technique/balise-meta-description/?utm_source=google&amp;utm_medium=orixa-site&amp;gclid=CjwKCAjwhaaKBhBcEiwA8acsHGvULoJNUxZxReWYFnntQHjFM_BnKldrTaUi-9S0kcUfg1C5bt3uSxoCO1EQAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-title/</t>
+  </si>
+  <si>
+    <t>https://black.bird.eu/fr/blog/performances-accelerer-le-chargement-des-images-sur-magento-2.html</t>
+  </si>
+  <si>
+    <t>https://blog.hubspot.fr/marketing/reduire-duree-chargement-page-web</t>
+  </si>
+  <si>
+    <t>https://fr.semrush.com/blog/texte-alternatif/</t>
+  </si>
+  <si>
+    <t>https://www.tech-wiki.online/fr/javascript-async-defer.html</t>
+  </si>
+  <si>
+    <t>https://maxime-benard.fr/article/42/fichier-htaccess-a-quoi-ca-sert</t>
+  </si>
+  <si>
+    <t>https://minifier.org/</t>
+  </si>
+  <si>
+    <t>https://fr.ryte.com/magazine/utiliser-mise-cache-navigateur-accelerer-site-web</t>
+  </si>
+  <si>
+    <t>http://www.pompage.net/traduction/Bien-utiliser-le-texte-alternatif</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Global_attributes/lang</t>
+  </si>
+  <si>
+    <t>https://wbcreation.fr/normes-w3c.html</t>
   </si>
 </sst>
 </file>
@@ -553,7 +589,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -604,7 +640,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -621,7 +657,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>77</v>
@@ -667,7 +703,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>77</v>
@@ -690,7 +726,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>77</v>
@@ -713,7 +749,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>77</v>
@@ -736,7 +772,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>77</v>
@@ -759,7 +795,7 @@
         <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>77</v>
@@ -782,7 +818,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>77</v>
@@ -805,7 +841,7 @@
         <v>44</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>77</v>
@@ -828,7 +864,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>77</v>
@@ -851,7 +887,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>77</v>
@@ -874,7 +910,7 @@
         <v>56</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>77</v>
@@ -897,7 +933,7 @@
         <v>59</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>77</v>
@@ -920,7 +956,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>77</v>
@@ -943,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>77</v>
@@ -989,7 +1025,7 @@
         <v>75</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>77</v>
@@ -1987,8 +2023,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F5" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile"/>
-    <hyperlink ref="F6:F18" r:id="rId3" display="https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile"/>
+    <hyperlink ref="F12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Amélioration du css pour le css validator
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>Catégorie</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>https://wbcreation.fr/normes-w3c.html</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
   </si>
 </sst>
 </file>
@@ -588,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -665,7 +668,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
@@ -987,7 +990,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Amélioration du rapport d'erreurs
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="30" windowWidth="17415" windowHeight="8115"/>
+    <workbookView xWindow="945" yWindow="615" windowWidth="27855" windowHeight="17385" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
     </ext>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Catégorie</t>
   </si>
@@ -39,6 +45,81 @@
     <t>Référence</t>
   </si>
   <si>
+    <t>La langue est mise sur "Default"</t>
+  </si>
+  <si>
+    <t>Si la langue est mise sur defaut alors le texte ne sera pas forcement en français</t>
+  </si>
+  <si>
+    <t>Il faut toujours mettre une ou plusieurs langues à son site</t>
+  </si>
+  <si>
+    <t>Renseigner la langue du site correctement</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-lang-why.fr</t>
+  </si>
+  <si>
+    <t>seo</t>
+  </si>
+  <si>
+    <t>Il manque la balise meta "robots index, follow" sur l'index et la page2</t>
+  </si>
+  <si>
+    <t>Il manque une balise importante dans le head qui permet aux robots de google d'indexer la page</t>
+  </si>
+  <si>
+    <t>Il faut toujours ajouter cette balise sur les pages qui doivent êtres indexées</t>
+  </si>
+  <si>
+    <t>Ajouter la balise</t>
+  </si>
+  <si>
+    <t>https://www.orixa-media.com/academie/referencement-naturel/technique/balise-meta-description/?utm_source=google&amp;utm_medium=orixa-site&amp;gclid=CjwKCAjwhaaKBhBcEiwA8acsHGvULoJNUxZxReWYFnntQHjFM_BnKldrTaUi-9S0kcUfg1C5bt3uSxoCO1EQAvD_BwE</t>
+  </si>
+  <si>
+    <t>Balise apparente</t>
+  </si>
+  <si>
+    <t>Au niveau de la nav barre du "bloc-0" on peut apperçevoir une balise apparente qui est liée à un problème de syntax</t>
+  </si>
+  <si>
+    <t>Les balises ne doivent pas apparaitrent sur les pages clients, il faut donc résoudre le problème de syntax pour la faire disparaitre</t>
+  </si>
+  <si>
+    <t>Enlever le "&amp;gt;" pour faire disparaitre cette balise</t>
+  </si>
+  <si>
+    <t>https://tim.cgmatane.qc.ca/charettes/conception-de-sites-web/les-bonnes-pratiques-du-html-5/</t>
+  </si>
+  <si>
+    <t>Le site web ne rescpecte pas les normes du W3C validator</t>
+  </si>
+  <si>
+    <t>Il y a des erreurs diverses à  peu près partout sur le site d'ordre sémantique, mauvais emploie de balisage</t>
+  </si>
+  <si>
+    <t>Il faut toujours respecter les normes du W3C car il représente les fondements du web</t>
+  </si>
+  <si>
+    <t>Corriger les erreurs misent en avant par le validateur</t>
+  </si>
+  <si>
+    <t>https://www.agenceici.com/le-blog/article/les-sites-web-se-doivent-de-respecter-la-norme-w3c-73</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>Pas de titre d'onglet</t>
+  </si>
+  <si>
     <t>Ce problème est lié à la balise "title" dans le code HTML5. Il faut ajouter un titre dans cette balise</t>
   </si>
   <si>
@@ -48,40 +129,67 @@
     <t>Ajout d'un titre accrocheur dans la balise title.</t>
   </si>
   <si>
-    <t>Balise apparente</t>
-  </si>
-  <si>
-    <t>Pas de titre d'onglet</t>
-  </si>
-  <si>
-    <t>Au niveau de la nav barre du "bloc-0" on peut apperçevoir une balise apparente qui est liée à un problème de syntax</t>
-  </si>
-  <si>
-    <t>Les balises ne doivent pas apparaitrent sur les pages clients, il faut donc résoudre le problème de syntax pour la faire disparaitre</t>
-  </si>
-  <si>
-    <t>Enlever le "&amp;gt;" pour faire disparaitre cette balise</t>
+    <t>https://smartkeyword.io/seo-on-page-balise-title/</t>
+  </si>
+  <si>
+    <t>Le temps de chargement du site est trop long</t>
+  </si>
+  <si>
+    <t>Il n' y a pas de compression de ressources, les fichiers sont donc trop lourds, ce qui ralentit le site web</t>
+  </si>
+  <si>
+    <t>La bonne pratique est de compresser les fichiers pour "alléger" le chargement du site</t>
+  </si>
+  <si>
+    <t>Il faut créer un fichier ".htacces" et paramétrer le GZIP pour effectuer la compression.</t>
+  </si>
+  <si>
+    <t>https://maxime-benard.fr/article/42/fichier-htaccess-a-quoi-ca-sert</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de mise en cache</t>
+  </si>
+  <si>
+    <t>Quand les visiteurs viennent pour la première fois sur le site il n'y a aucune sauvegarde automatique des données car il n' y a aucun cache navigateur. Ce qui fais que les visiteurs sont obligés de retélécharger les données à chaque fois qu'ils reviendront.</t>
+  </si>
+  <si>
+    <t>Le mieux est de rajouter un cache navigateur pour s'éviter ce désagrémant</t>
+  </si>
+  <si>
+    <t>Le mieux est d'utiliser les deux méthodes de cache car elles sont complémentaires. La méthode "Cache-contrôle" sera prioritaire toute fois.</t>
+  </si>
+  <si>
+    <t>https://fr.ryte.com/magazine/utiliser-mise-cache-navigateur-accelerer-site-web</t>
   </si>
   <si>
     <t>Images démesurées</t>
   </si>
   <si>
+    <t>Les images "1.jpg" et "2.jpg" sont trop grandes par rapport à leurs conteneurs</t>
+  </si>
+  <si>
     <t>Il faut toujours faire en sorte d'approcher la taille des images par rapport à la taille des conteneurs dans lesquels elles seront stockées</t>
   </si>
   <si>
     <t>Réduire la taille de ces deux images pour fludifier le chargement de la page web.</t>
   </si>
   <si>
-    <t>SEO</t>
-  </si>
-  <si>
-    <t>seo &amp; accessibilité</t>
-  </si>
-  <si>
-    <t>seo</t>
-  </si>
-  <si>
-    <t>Les images "1.jpg" et "2.jpg" sont trop grandes par rapport à leurs conteneurs</t>
+    <t>https://blog.hubspot.fr/marketing/reduire-duree-chargement-page-web</t>
+  </si>
+  <si>
+    <t>Les fichiers JS et CSS ne sont pas minifiés</t>
+  </si>
+  <si>
+    <t>Il y a des caractères inutiles dans ces fichiers comme par exemples les espaces et les sauts de lignes ce qui augmente le poids des fichiers inutilement.</t>
+  </si>
+  <si>
+    <t>Il faut réduire se poid en enlevant tous ces caractères inutiles</t>
+  </si>
+  <si>
+    <t>Le mieux est de passer par un logiciel de minisation de fichiers tel que: minifier.org</t>
+  </si>
+  <si>
+    <t>https://minifier.org/</t>
   </si>
   <si>
     <t>La bannière et les images "1.jpg" et "2.jpg" sont trop lourdes</t>
@@ -96,76 +204,37 @@
     <t>Compresser les images tout en gardant le format adpater et la qualitée de l'image</t>
   </si>
   <si>
-    <t>Mauvaise description des textes alternatifs sur les images "1,2,3,4.jpg/bmp"</t>
-  </si>
-  <si>
-    <t>Le texte alternatif n'est pas clair, trop long et ne met pas en avant la chouette agence</t>
-  </si>
-  <si>
-    <t>Le texte alternatif doit être le plus clair possible pour les personnes aveugles ou mal voyantes, il faut donc un texte court et facilement compréhensible. Qui plus est, le texte doit mettre l'agence en avant en utilisant des "mot-clés" pour optimiser le référencement naturel</t>
-  </si>
-  <si>
-    <t>Changer le texte alternatif de façon à ce qu'il soit plus clair et qu'il mette la chouette agence en avant sur les pages de Google</t>
+    <t>https://black.bird.eu/fr/blog/performances-accelerer-le-chargement-des-images-sur-magento-2.html</t>
   </si>
   <si>
     <t xml:space="preserve">L'appel des fichiers JS ne se fais pas correctement. </t>
   </si>
   <si>
+    <t>Il n'y a pas d'exécution particulière pour les fichiers JS, cela peut bloquer l'affichage de la page durant le temps de leurs chargements.</t>
+  </si>
+  <si>
     <t>Il faut (dans le cas ou le JS est utilisé pour sublimer la page) soit faire une exécution "asynchrone" ou alors une "différée"</t>
   </si>
   <si>
-    <t>Il n'y a pas d'exécution particulière pour les fichiers JS, cela peut bloquer l'affichage de la page durant le temps de leurs chargements.</t>
-  </si>
-  <si>
     <t>Ici le mieux serai de faire une exécution "différée" pour que les scripts se lancent dès que le HTML aura finit de se charger</t>
   </si>
   <si>
-    <t>Le temps de chargement du site est trop long</t>
-  </si>
-  <si>
-    <t>La bonne pratique est de compresser les fichiers pour "alléger" le chargement du site</t>
-  </si>
-  <si>
-    <t>Il faut créer un fichier ".htacces" et paramétrer le GZIP pour effectuer la compression.</t>
-  </si>
-  <si>
-    <t>Il n' y a pas de compression de ressources, les fichiers sont donc trop lourds, ce qui ralentit le site web</t>
-  </si>
-  <si>
-    <t>Les fichiers JS et CSS ne sont pas minifiés</t>
-  </si>
-  <si>
-    <t>Il y a des caractères inutiles dans ces fichiers comme par exemples les espaces et les sauts de lignes ce qui augmente le poids des fichiers inutilement.</t>
-  </si>
-  <si>
-    <t>Il faut réduire se poid en enlevant tous ces caractères inutiles</t>
-  </si>
-  <si>
-    <t>Le mieux est de passer par un logiciel de minisation de fichiers tel que: minifier.org</t>
-  </si>
-  <si>
-    <t>Il n'y a pas de mise en cache</t>
-  </si>
-  <si>
-    <t>Quand les visiteurs viennent pour la première fois sur le site il n'y a aucune sauvegarde automatique des données car il n' y a aucun cache navigateur. Ce qui fais que les visiteurs sont obligés de retélécharger les données à chaque fois qu'ils reviendront.</t>
-  </si>
-  <si>
-    <t>Le mieux est de rajouter un cache navigateur pour s'éviter ce désagrémant</t>
-  </si>
-  <si>
-    <t>Le mieux est d'utiliser les deux méthodes de cache car elles sont complémentaires. La méthode "Cache-contrôle" sera prioritaire toute fois.</t>
-  </si>
-  <si>
-    <t>Les textes alternatifs ne respect pas les principaux mot-clés</t>
-  </si>
-  <si>
-    <t>La Chouette agence web se trouve à Lyon, il faut mettre en avant cela. Dans beaucoup de textes alternatifs il y a marqué "agence web à Paris".</t>
-  </si>
-  <si>
-    <t>Les textes alternatifs doivent reprendre les principaux mot-clés, il faut donc reprendre les mot-clés suivants: “Entreprise web design Lyon”</t>
-  </si>
-  <si>
-    <t>Intégrer les bons mot-clés dans les textes alternatifs</t>
+    <t>https://www.tech-wiki.online/fr/javascript-async-defer.html</t>
+  </si>
+  <si>
+    <t>Images non responsives</t>
+  </si>
+  <si>
+    <t>Certaines images ne sont pas adaptées au format smartphone</t>
+  </si>
+  <si>
+    <t>Il faut toujours qu'un site web puisse s'adapter aux différents écrans, il faut donc apporter des modifications au niveau du breakpoint du format smartphone</t>
+  </si>
+  <si>
+    <t>Ici le mieux est de mettre la largeur de l'image à 100% ce qui l'obligera à respecter la largeur imposée par le breakpoint du smartphone.</t>
+  </si>
+  <si>
+    <t>https://www.ideagency.fr/blog/responsive-design-ux</t>
   </si>
   <si>
     <t>Une balise meta n'est pas complétée dans le head de l'index.html</t>
@@ -180,125 +249,20 @@
     <t>Remplir la partie content</t>
   </si>
   <si>
-    <t>La langue est mise sur "Default"</t>
-  </si>
-  <si>
-    <t>Si la langue est mise sur defaut alors le texte ne sera pas forcement en français</t>
-  </si>
-  <si>
-    <t>Il faut toujours mettre une ou plusieurs langues à son site</t>
-  </si>
-  <si>
-    <t>Renseigner la langue du site correctement</t>
-  </si>
-  <si>
-    <t>Il manque une balise importante dans le head qui permet aux robots de google d'indexer la page</t>
-  </si>
-  <si>
-    <t>Il faut toujours ajouter cette balise sur les pages qui doivent êtres indexées</t>
-  </si>
-  <si>
-    <t>Ajouter la balise</t>
-  </si>
-  <si>
-    <t>Il faut remplir la partie "content" sur la balise meta description et keywords sinon le google bot ne pourra pas comprendre</t>
-  </si>
-  <si>
-    <t>Il faut toujours remplir la partie "content" des balises pour augmenter son référencement naturel</t>
-  </si>
-  <si>
-    <t>Les parties "content" des balises keyword et description ne sont pas remplies sur la page2.</t>
-  </si>
-  <si>
-    <t>Il manque la balise meta "robots index, follow" sur l'index et la page2</t>
-  </si>
-  <si>
-    <t>Le texte alternatif du logo de la chouette agence a une mauvaise description</t>
-  </si>
-  <si>
-    <t>Le texte alternatif doit mettre en avant l'agence de lyon et en l'occurrence ici il parle d'atlanta</t>
-  </si>
-  <si>
-    <t>Il faut toujours faire en sorte que le texte alt reprenne les mot-clés pour optimiser le référencement naturel</t>
-  </si>
-  <si>
-    <t>Enlever le "atlanta" par "lyon"</t>
-  </si>
-  <si>
-    <t>La navigation n'est presque pas visible sur la page 2</t>
-  </si>
-  <si>
-    <t>Tout contenu doit être visible pour les visiteurs du site web</t>
-  </si>
-  <si>
-    <t>Recentrer la navigation</t>
-  </si>
-  <si>
-    <t>Reprendre le code CSS pour faire en sorte que la navigation soit au milieu</t>
-  </si>
-  <si>
-    <t>Le site web ne rescpecte pas les normes du W3C validator</t>
-  </si>
-  <si>
-    <t>Il y a des erreurs diverses à  peu près partout sur le site d'ordre sémantique, mauvais emploie de balisage</t>
-  </si>
-  <si>
-    <t>Il faut toujours respecter les normes du W3C car il représente les fondements du web</t>
-  </si>
-  <si>
-    <t>Corriger les erreurs misent en avant par le validateur</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>https://www.orixa-media.com/academie/referencement-naturel/technique/balise-meta-description/?utm_source=google&amp;utm_medium=orixa-site&amp;gclid=CjwKCAjwhaaKBhBcEiwA8acsHGvULoJNUxZxReWYFnntQHjFM_BnKldrTaUi-9S0kcUfg1C5bt3uSxoCO1EQAvD_BwE</t>
-  </si>
-  <si>
-    <t>https://smartkeyword.io/seo-on-page-balise-title/</t>
-  </si>
-  <si>
-    <t>https://black.bird.eu/fr/blog/performances-accelerer-le-chargement-des-images-sur-magento-2.html</t>
-  </si>
-  <si>
-    <t>https://blog.hubspot.fr/marketing/reduire-duree-chargement-page-web</t>
-  </si>
-  <si>
-    <t>https://fr.semrush.com/blog/texte-alternatif/</t>
-  </si>
-  <si>
-    <t>https://www.tech-wiki.online/fr/javascript-async-defer.html</t>
-  </si>
-  <si>
-    <t>https://maxime-benard.fr/article/42/fichier-htaccess-a-quoi-ca-sert</t>
-  </si>
-  <si>
-    <t>https://minifier.org/</t>
-  </si>
-  <si>
-    <t>https://fr.ryte.com/magazine/utiliser-mise-cache-navigateur-accelerer-site-web</t>
-  </si>
-  <si>
-    <t>http://www.pompage.net/traduction/Bien-utiliser-le-texte-alternatif</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Global_attributes/lang</t>
-  </si>
-  <si>
-    <t>https://wbcreation.fr/normes-w3c.html</t>
-  </si>
-  <si>
-    <t>accessibilité</t>
+    <t>Le site web ne rescpecte pas les normes du W3C CSS validator</t>
+  </si>
+  <si>
+    <t>Il y a des erreurs diverses à  peu près partout sur le site au niveau du css.</t>
+  </si>
+  <si>
+    <t>https://openweb.eu.org/articles/pourquoi_standards/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,16 +273,20 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -330,6 +298,10 @@
       <sz val="10.45"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -364,30 +336,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -591,14 +571,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
@@ -643,418 +623,345 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>76</v>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>81</v>
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>82</v>
+      <c r="A6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>83</v>
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>85</v>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>86</v>
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>87</v>
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>78</v>
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>88</v>
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>78</v>
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>77</v>
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2025,8 +1932,14 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F12" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
+    <hyperlink ref="F9" r:id="rId4"/>
+    <hyperlink ref="F11" r:id="rId5"/>
+    <hyperlink ref="F14" r:id="rId6"/>
+    <hyperlink ref="F4" r:id="rId7"/>
+    <hyperlink ref="F15" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Résolution du problème de SEO concernant les keywords répétitives et changement du nom de la page2 en contact
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1940,6 +1940,12 @@
     <hyperlink ref="F14" r:id="rId6"/>
     <hyperlink ref="F4" r:id="rId7"/>
     <hyperlink ref="F15" r:id="rId8"/>
+    <hyperlink ref="F2" r:id="rId9"/>
+    <hyperlink ref="F5" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="F8" r:id="rId12"/>
+    <hyperlink ref="F12" r:id="rId13"/>
+    <hyperlink ref="F13" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Mise à jour du rapport d'erreurs et du rapport d'optimisation
</commit_message>
<xml_diff>
--- a/Releve_erreur.xlsx
+++ b/Releve_erreur.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>Catégorie</t>
   </si>
@@ -99,21 +99,6 @@
     <t>https://tim.cgmatane.qc.ca/charettes/conception-de-sites-web/les-bonnes-pratiques-du-html-5/</t>
   </si>
   <si>
-    <t>Le site web ne rescpecte pas les normes du W3C validator</t>
-  </si>
-  <si>
-    <t>Il y a des erreurs diverses à  peu près partout sur le site d'ordre sémantique, mauvais emploie de balisage</t>
-  </si>
-  <si>
-    <t>Il faut toujours respecter les normes du W3C car il représente les fondements du web</t>
-  </si>
-  <si>
-    <t>Corriger les erreurs misent en avant par le validateur</t>
-  </si>
-  <si>
-    <t>https://www.agenceici.com/le-blog/article/les-sites-web-se-doivent-de-respecter-la-norme-w3c-73</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -207,36 +192,6 @@
     <t>https://black.bird.eu/fr/blog/performances-accelerer-le-chargement-des-images-sur-magento-2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">L'appel des fichiers JS ne se fais pas correctement. </t>
-  </si>
-  <si>
-    <t>Il n'y a pas d'exécution particulière pour les fichiers JS, cela peut bloquer l'affichage de la page durant le temps de leurs chargements.</t>
-  </si>
-  <si>
-    <t>Il faut (dans le cas ou le JS est utilisé pour sublimer la page) soit faire une exécution "asynchrone" ou alors une "différée"</t>
-  </si>
-  <si>
-    <t>Ici le mieux serai de faire une exécution "différée" pour que les scripts se lancent dès que le HTML aura finit de se charger</t>
-  </si>
-  <si>
-    <t>https://www.tech-wiki.online/fr/javascript-async-defer.html</t>
-  </si>
-  <si>
-    <t>Images non responsives</t>
-  </si>
-  <si>
-    <t>Certaines images ne sont pas adaptées au format smartphone</t>
-  </si>
-  <si>
-    <t>Il faut toujours qu'un site web puisse s'adapter aux différents écrans, il faut donc apporter des modifications au niveau du breakpoint du format smartphone</t>
-  </si>
-  <si>
-    <t>Ici le mieux est de mettre la largeur de l'image à 100% ce qui l'obligera à respecter la largeur imposée par le breakpoint du smartphone.</t>
-  </si>
-  <si>
-    <t>https://www.ideagency.fr/blog/responsive-design-ux</t>
-  </si>
-  <si>
     <t>Une balise meta n'est pas complétée dans le head de l'index.html</t>
   </si>
   <si>
@@ -249,13 +204,97 @@
     <t>Remplir la partie content</t>
   </si>
   <si>
-    <t>Le site web ne rescpecte pas les normes du W3C CSS validator</t>
-  </si>
-  <si>
-    <t>Il y a des erreurs diverses à  peu près partout sur le site au niveau du css.</t>
-  </si>
-  <si>
-    <t>https://openweb.eu.org/articles/pourquoi_standards/</t>
+    <t>Les couleurs ne sont pas assez nettes pour certaines personnes mal voyantes</t>
+  </si>
+  <si>
+    <t>Il faut respecter les normes de l'accessibilité en utilisant des couleurs visibles même pour des gens mals voyants</t>
+  </si>
+  <si>
+    <t>Il faut changer les couleurs pour quel soient plus visibles</t>
+  </si>
+  <si>
+    <t>Changer les couleurs des font pour les faire ressortir par rapport au background et également augmenter la taille des polices si cela est nécessaire</t>
+  </si>
+  <si>
+    <t>https://blog.ipedis.com/accessibilite-web-normes-et-bonnes-pratiques-a-respecter</t>
+  </si>
+  <si>
+    <t>accessibilité &amp; SEO</t>
+  </si>
+  <si>
+    <t>Il y a des images qui représentent du texte</t>
+  </si>
+  <si>
+    <t>Les images ont un but esthétique, d'information, mais surement pas de montrer du texte</t>
+  </si>
+  <si>
+    <t>Il faut utiliser des images à des fins esthétique, d'information, marketing pas pour autre chose</t>
+  </si>
+  <si>
+    <t>Remplacer les images qui représente du texte par du vrai texte</t>
+  </si>
+  <si>
+    <t>https://www.webetsolutions.com/blog/le-pouvoir-des-images-pour-site-web/</t>
+  </si>
+  <si>
+    <t>Il n y a pas de balise gtag</t>
+  </si>
+  <si>
+    <t>La balise gtag permet de faire la liason avec google analytics, si le gtag est absent on ne pourra pas collerter les données sur les visiteurs</t>
+  </si>
+  <si>
+    <t>Il faut toujours mettre la balise gtag pour pouvoir se servir de google analytics</t>
+  </si>
+  <si>
+    <t>Ajouter la balise gtag pour pouvoir collerter les données des visiteurs sur google analytics</t>
+  </si>
+  <si>
+    <t>https://angulaire.io/blog/google-tag-manager</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de balises de structure du HTML</t>
+  </si>
+  <si>
+    <t>Les balises de structure sont absentes, ce qui est un vrai problème pour les normes du W3C</t>
+  </si>
+  <si>
+    <t>Il faut toujours utiliser les balises de structure du html pour respecter les bonnes pratiques du web.</t>
+  </si>
+  <si>
+    <t>Rajouter les bonnes balises de structure (header, main, section, etc…)</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
+  </si>
+  <si>
+    <t>Des mot clés sont utilisés de manière abusive</t>
+  </si>
+  <si>
+    <t>Les mot clés ne doivent pas êtres utilisés de façon abusive inutilement cela me provocer un "black hat"</t>
+  </si>
+  <si>
+    <t>Les mot clés doivent être utiliser dans des endroits spécifique comme dans les titres et une seul fois au même endroit</t>
+  </si>
+  <si>
+    <t>Retirer les balises keywords ou les mot clés sont utilisés de manière abusive pour éviter le sanctionnement de google. Il faut plutôt se tourner vair une pratique de white hat.</t>
+  </si>
+  <si>
+    <t>https://www.semjuice.com/definition/black-hat-seo?gclid=CjwKCAjw-sqKBhBjEiwAVaQ9a26E9b64rzuXrffH4EbhCJcui1X_jkB39IwKS3jD9D7PhnQAiW-IWhoCG5YQAvD_BwE</t>
+  </si>
+  <si>
+    <t>Il manque des aria-label à certains endroits</t>
+  </si>
+  <si>
+    <t>Les aria-label sont très importants pour des utilisateurs mals voyants ou aveugles car ils permettent de lire des éléments ou la lecture du texte n'est pas possible.</t>
+  </si>
+  <si>
+    <t>Il faut toujours ajouter des aria-labels sur des éléments dépourvus de textes pour que le contenu du site soit accessible à tous types d'utilisateurs.</t>
+  </si>
+  <si>
+    <t>Rajouter des aria-labels aux endroits nécessaire comme les icônes des réseaux sociaux ou encore sur le bouton du menu de navigation en mode smartphone.</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/ARIA/ARIA_Techniques/Using_the_aria-label_attribute</t>
   </si>
 </sst>
 </file>
@@ -341,7 +380,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,6 +395,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -572,7 +613,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A20" sqref="A20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -674,16 +715,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>18</v>
@@ -717,22 +758,22 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>10</v>
@@ -743,19 +784,19 @@
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>10</v>
@@ -831,23 +872,23 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>54</v>
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>10</v>
@@ -858,42 +899,42 @@
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>64</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>10</v>
@@ -901,67 +942,141 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>76</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1933,19 +2048,21 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F7" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F11" r:id="rId5"/>
-    <hyperlink ref="F14" r:id="rId6"/>
-    <hyperlink ref="F4" r:id="rId7"/>
-    <hyperlink ref="F15" r:id="rId8"/>
-    <hyperlink ref="F2" r:id="rId9"/>
-    <hyperlink ref="F5" r:id="rId10"/>
-    <hyperlink ref="F10" r:id="rId11"/>
-    <hyperlink ref="F8" r:id="rId12"/>
-    <hyperlink ref="F12" r:id="rId13"/>
-    <hyperlink ref="F13" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+    <hyperlink ref="F10" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="F2" r:id="rId6"/>
+    <hyperlink ref="F5" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F7" r:id="rId9"/>
+    <hyperlink ref="F12" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>